<commit_message>
Update status and tasks
</commit_message>
<xml_diff>
--- a/Documentation/Project1TaskSpreadsheet.xlsx
+++ b/Documentation/Project1TaskSpreadsheet.xlsx
@@ -19,7 +19,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
+  <si>
+    <t>Write GUI for controlling movement of the Vex</t>
+  </si>
+  <si>
+    <t>Test movement GUI</t>
+  </si>
+  <si>
+    <t>Ensure efficient motor control algorithm</t>
+  </si>
+  <si>
+    <t>Test robot moving forward/back/left/right on 10% grade</t>
+  </si>
+  <si>
+    <t>Read documentation on Vex controller communication</t>
+  </si>
+  <si>
+    <t>Use Bump Sensors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>May need to do some mechanical fixes for making sure the wheels rotate smoothly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create main application loop listening for input</t>
+  </si>
+  <si>
+    <t>Test reception of static speed parameter inputs</t>
+  </si>
+  <si>
+    <t>Calibrate speed based on joystick position</t>
+  </si>
+  <si>
+    <t>Modify control loop for dynamic speed</t>
+  </si>
+  <si>
+    <t>Test dynamic speeds</t>
+  </si>
   <si>
     <t>Modify control loop to allow turning while moving</t>
   </si>
@@ -184,36 +222,6 @@
   </si>
   <si>
     <t>Test communication code</t>
-  </si>
-  <si>
-    <t>Write GUI for controlling movement of the Vex</t>
-  </si>
-  <si>
-    <t>Test movement GUI</t>
-  </si>
-  <si>
-    <t>Ensure efficient motor control algorithm</t>
-  </si>
-  <si>
-    <t>Test robot moving forward/back/left/right on 10% grade</t>
-  </si>
-  <si>
-    <t>Read documentation on Vex controller communication</t>
-  </si>
-  <si>
-    <t>Create main application loop listening for input</t>
-  </si>
-  <si>
-    <t>Test reception of static speed parameter inputs</t>
-  </si>
-  <si>
-    <t>Calibrate speed based on joystick position</t>
-  </si>
-  <si>
-    <t>Modify control loop for dynamic speed</t>
-  </si>
-  <si>
-    <t>Test dynamic speeds</t>
   </si>
 </sst>
 </file>
@@ -705,7 +713,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -718,37 +726,37 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H1" s="7">
         <f ca="1">TODAY()</f>
-        <v>40061</v>
+        <v>40062</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5">
         <v>40059</v>
@@ -767,10 +775,10 @@
     </row>
     <row r="3" spans="1:8" ht="14" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5">
         <v>40059</v>
@@ -789,10 +797,10 @@
     </row>
     <row r="4" spans="1:8" ht="14" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5">
         <v>40059</v>
@@ -811,10 +819,10 @@
     </row>
     <row r="5" spans="1:8" ht="14" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5">
         <v>40059</v>
@@ -831,10 +839,10 @@
     </row>
     <row r="6" spans="1:8" ht="14" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5">
         <v>40059</v>
@@ -853,10 +861,10 @@
     </row>
     <row r="7" spans="1:8" ht="14" thickBot="1">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5">
         <v>40060</v>
@@ -875,10 +883,10 @@
     </row>
     <row r="8" spans="1:8" ht="14" thickBot="1">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5">
         <v>40060</v>
@@ -897,10 +905,10 @@
     </row>
     <row r="9" spans="1:8" ht="14" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5">
         <v>40061</v>
@@ -919,10 +927,10 @@
     </row>
     <row r="10" spans="1:8" ht="14" thickBot="1">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5">
         <v>40061</v>
@@ -934,15 +942,15 @@
       <c r="F10" s="6"/>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C11" s="5">
         <v>40061</v>
@@ -954,15 +962,15 @@
       <c r="F11" s="6"/>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14" thickBot="1">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C12" s="5">
         <v>40061</v>
@@ -974,15 +982,15 @@
       <c r="F12" s="6"/>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14" thickBot="1">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5">
         <v>40061</v>
@@ -994,15 +1002,15 @@
       <c r="F13" s="6"/>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14" thickBot="1">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5">
         <v>40061</v>
@@ -1021,10 +1029,10 @@
     </row>
     <row r="15" spans="1:8" ht="14" thickBot="1">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C15" s="5">
         <v>40061</v>
@@ -1043,10 +1051,10 @@
     </row>
     <row r="16" spans="1:8" ht="14" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5">
         <v>40063</v>
@@ -1063,13 +1071,13 @@
     </row>
     <row r="17" spans="1:7" ht="14" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D17" s="13">
         <v>0</v>
@@ -1083,18 +1091,20 @@
     </row>
     <row r="18" spans="1:7" ht="14" thickBot="1">
       <c r="A18" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5">
         <v>40063</v>
       </c>
       <c r="D18" s="13">
-        <v>0</v>
-      </c>
-      <c r="E18" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="9">
+        <v>40062</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18">
         <f t="shared" ca="1" si="0"/>
@@ -1103,10 +1113,10 @@
     </row>
     <row r="19" spans="1:7" ht="14" thickBot="1">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C19" s="5">
         <v>40061</v>
@@ -1125,18 +1135,20 @@
     </row>
     <row r="20" spans="1:7" ht="14" thickBot="1">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C20" s="5">
         <v>40063</v>
       </c>
       <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="9">
+        <v>40062</v>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20">
         <f t="shared" ca="1" si="0"/>
@@ -1145,18 +1157,20 @@
     </row>
     <row r="21" spans="1:7" ht="14" thickBot="1">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C21" s="5">
         <v>40063</v>
       </c>
       <c r="D21" s="13">
-        <v>0</v>
-      </c>
-      <c r="E21" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="9">
+        <v>40062</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21">
         <f t="shared" ca="1" si="0"/>
@@ -1165,18 +1179,20 @@
     </row>
     <row r="22" spans="1:7" ht="14" thickBot="1">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C22" s="5">
         <v>40063</v>
       </c>
       <c r="D22" s="13">
-        <v>0</v>
-      </c>
-      <c r="E22" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="9">
+        <v>40062</v>
+      </c>
       <c r="F22" s="6"/>
       <c r="G22">
         <f t="shared" ca="1" si="0"/>
@@ -1185,18 +1201,20 @@
     </row>
     <row r="23" spans="1:7" ht="14" thickBot="1">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C23" s="5">
         <v>40063</v>
       </c>
       <c r="D23" s="13">
-        <v>0</v>
-      </c>
-      <c r="E23" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="9">
+        <v>40062</v>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23">
         <f t="shared" ca="1" si="0"/>
@@ -1205,19 +1223,23 @@
     </row>
     <row r="24" spans="1:7" ht="14" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C24" s="5">
         <v>40063</v>
       </c>
       <c r="D24" s="13">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="9">
+        <v>40062</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="G24">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
@@ -1225,18 +1247,20 @@
     </row>
     <row r="25" spans="1:7" ht="14" thickBot="1">
       <c r="A25" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C25" s="5">
         <v>40063</v>
       </c>
       <c r="D25" s="13">
-        <v>0</v>
-      </c>
-      <c r="E25" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="9">
+        <v>40062</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25">
         <f t="shared" ca="1" si="0"/>
@@ -1245,19 +1269,23 @@
     </row>
     <row r="26" spans="1:7" ht="14" thickBot="1">
       <c r="A26" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C26" s="5">
         <v>40066</v>
       </c>
       <c r="D26" s="13">
-        <v>0</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>40062</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="G26">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
@@ -1265,10 +1293,10 @@
     </row>
     <row r="27" spans="1:7" ht="14" thickBot="1">
       <c r="A27" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C27" s="5">
         <v>40066</v>
@@ -1285,10 +1313,10 @@
     </row>
     <row r="28" spans="1:7" ht="14" thickBot="1">
       <c r="A28" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C28" s="5">
         <v>40069</v>
@@ -1305,10 +1333,10 @@
     </row>
     <row r="29" spans="1:7" ht="14" thickBot="1">
       <c r="A29" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C29" s="5">
         <v>40070</v>
@@ -1325,10 +1353,10 @@
     </row>
     <row r="30" spans="1:7" ht="14" thickBot="1">
       <c r="A30" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C30" s="5">
         <v>40061</v>
@@ -1340,15 +1368,15 @@
       <c r="F30" s="6"/>
       <c r="G30">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14" thickBot="1">
       <c r="A31" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C31" s="5">
         <v>40066</v>
@@ -1365,10 +1393,10 @@
     </row>
     <row r="32" spans="1:7" ht="14" thickBot="1">
       <c r="A32" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C32" s="5">
         <v>40069</v>
@@ -1385,10 +1413,10 @@
     </row>
     <row r="33" spans="1:7" ht="14" thickBot="1">
       <c r="A33" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C33" s="5">
         <v>40070</v>
@@ -1405,10 +1433,10 @@
     </row>
     <row r="34" spans="1:7" ht="14" thickBot="1">
       <c r="A34" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C34" s="5">
         <v>40061</v>
@@ -1420,15 +1448,15 @@
       <c r="F34" s="6"/>
       <c r="G34">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="14" thickBot="1">
       <c r="A35" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C35" s="5">
         <v>40066</v>
@@ -1445,10 +1473,10 @@
     </row>
     <row r="36" spans="1:7" ht="14" thickBot="1">
       <c r="A36" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C36" s="5">
         <v>40069</v>
@@ -1465,10 +1493,10 @@
     </row>
     <row r="37" spans="1:7" ht="14" thickBot="1">
       <c r="A37" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C37" s="5">
         <v>40070</v>
@@ -1485,10 +1513,10 @@
     </row>
     <row r="38" spans="1:7" ht="14" thickBot="1">
       <c r="A38" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="C38" s="5">
         <v>40073</v>
@@ -1505,10 +1533,10 @@
     </row>
     <row r="39" spans="1:7" ht="14" thickBot="1">
       <c r="A39" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C39" s="5">
         <v>40074</v>
@@ -1525,10 +1553,10 @@
     </row>
     <row r="40" spans="1:7" ht="14" thickBot="1">
       <c r="A40" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="C40" s="5">
         <v>40076</v>
@@ -1545,10 +1573,10 @@
     </row>
     <row r="41" spans="1:7" ht="14" thickBot="1">
       <c r="A41" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C41" s="5">
         <v>40076</v>
@@ -1565,10 +1593,10 @@
     </row>
     <row r="42" spans="1:7" ht="14" thickBot="1">
       <c r="A42" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="C42" s="5">
         <v>40063</v>
@@ -1585,10 +1613,10 @@
     </row>
     <row r="43" spans="1:7" ht="14" thickBot="1">
       <c r="A43" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C43" s="5">
         <v>40069</v>
@@ -1605,10 +1633,10 @@
     </row>
     <row r="44" spans="1:7" ht="14" thickBot="1">
       <c r="A44" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C44" s="5">
         <v>40069</v>
@@ -1625,10 +1653,10 @@
     </row>
     <row r="45" spans="1:7" ht="14" thickBot="1">
       <c r="A45" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="C45" s="5">
         <v>40073</v>
@@ -1645,10 +1673,10 @@
     </row>
     <row r="46" spans="1:7" ht="14" thickBot="1">
       <c r="A46" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="C46" s="5">
         <v>40073</v>
@@ -1665,10 +1693,10 @@
     </row>
     <row r="47" spans="1:7" ht="14" thickBot="1">
       <c r="A47" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="C47" s="5">
         <v>40075</v>
@@ -1685,10 +1713,10 @@
     </row>
     <row r="48" spans="1:7" ht="14" thickBot="1">
       <c r="A48" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C48" s="5">
         <v>40077</v>
@@ -1705,10 +1733,10 @@
     </row>
     <row r="49" spans="1:7" ht="14" thickBot="1">
       <c r="A49" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C49" s="5">
         <v>40077</v>
@@ -1725,10 +1753,10 @@
     </row>
     <row r="50" spans="1:7" ht="14" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C50" s="5">
         <v>40078</v>
@@ -1745,10 +1773,10 @@
     </row>
     <row r="51" spans="1:7" ht="14" thickBot="1">
       <c r="A51" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="C51" s="5">
         <v>40079</v>
@@ -1765,10 +1793,10 @@
     </row>
     <row r="52" spans="1:7" ht="14" thickBot="1">
       <c r="A52" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C52" s="5">
         <v>40079</v>
@@ -1784,6 +1812,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C52">
     <cfRule type="expression" dxfId="1" priority="0" stopIfTrue="1">

</xml_diff>